<commit_message>
notes to code chunk for Q4
</commit_message>
<xml_diff>
--- a/HW3Data.xlsx
+++ b/HW3Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamie K\Documents\UCSB\Spring 2019\ESM 204 Economics of Environmental Management\Assignments\Assignment 3\ESM204_HW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{42591345-F897-4155-9FA0-A5C84CE570AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2661926-95B5-4EBD-9159-94B41D84B06D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9504" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9504" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW3Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HW3Data!$L$2:$M$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HW3Data!$A$1:$F$501</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -88,13 +88,13 @@
     <t>Count of NEP</t>
   </si>
   <si>
-    <t>Count of income</t>
+    <t>Count of age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,7 +638,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jamie K" refreshedDate="43607.713714583333" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="501">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jamie K" refreshedDate="43607.713714583333" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="501" xr:uid="{00000000-000A-0000-FFFF-FFFF07000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="HW3Data"/>
   </cacheSource>
@@ -4765,7 +4765,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I2:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
@@ -4851,7 +4851,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
+    <pivotField showAll="0">
       <items count="7">
         <item x="1"/>
         <item x="2"/>
@@ -4862,7 +4862,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="7">
         <item x="4"/>
         <item x="2"/>
@@ -4875,7 +4875,7 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="4"/>
+    <field x="5"/>
   </rowFields>
   <rowItems count="7">
     <i>
@@ -4904,7 +4904,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of income" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of age" fld="5" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -5214,18 +5214,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I7" sqref="I7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -5300,10 +5299,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J3" s="3">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -5332,10 +5331,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J4" s="3">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="L4">
         <v>40</v>
@@ -5364,10 +5363,10 @@
         <v>7</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="3">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="L5">
         <v>41</v>
@@ -5396,10 +5395,10 @@
         <v>10</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J6" s="3">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="L6">
         <v>39</v>
@@ -5428,10 +5427,10 @@
         <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J7" s="3">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="L7">
         <v>32</v>
@@ -15598,11 +15597,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="L2:M52">
-    <sortState ref="L3:M52">
-      <sortCondition descending="1" ref="M2:M52"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:F501" xr:uid="{BD1A70D4-C22F-439E-8CD7-F0F625D34F7A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>